<commit_message>
seperate summary to outpatient and inpatient.
</commit_message>
<xml_diff>
--- a/mapping/mml_surgery_mapping.xlsx
+++ b/mapping/mml_surgery_mapping.xlsx
@@ -79,10 +79,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>mmlBc:BaseClinicModule</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mmlSg:SurgeryModule</t>
   </si>
   <si>
@@ -1334,6 +1330,10 @@
   </si>
   <si>
     <t>[openEHR-EHR-COMPOSITION.report-procedure.v1]/content[openEHR-EHR-EVALUATION.clinical_synopsis.v1 and name/value='Clinical Synopsis']/data[at0001]/items[at0002]/value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mmlSg:SurgeryModule</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1767,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C184" workbookViewId="0">
-      <selection activeCell="J197" sqref="J197"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>364</v>
       </c>
       <c r="B2" s="2"/>
       <c r="H2" t="s">
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1838,7 +1838,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1852,36 +1852,36 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
@@ -1889,16 +1889,16 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="I8" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
@@ -1906,18 +1906,18 @@
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="3"/>
       <c r="I9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
@@ -1925,21 +1925,21 @@
         <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="3"/>
       <c r="I10" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
@@ -1947,7 +1947,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1958,23 +1958,23 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="H12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
@@ -1985,45 +1985,45 @@
       </c>
       <c r="F13" s="3"/>
       <c r="I13" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="I14" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="J14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="3"/>
       <c r="I15" s="7"/>
@@ -2031,7 +2031,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
@@ -2042,92 +2042,92 @@
       </c>
       <c r="F16" s="3"/>
       <c r="I16" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="C17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="J17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="3"/>
       <c r="I19" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="C20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="I20" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="J20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2138,65 +2138,65 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="H22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="I23" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" s="3"/>
       <c r="I24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
@@ -2211,53 +2211,53 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="I26" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" s="3"/>
       <c r="I27" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -2265,48 +2265,48 @@
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I29" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="I30" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2315,13 +2315,13 @@
       </c>
       <c r="F31" s="3"/>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
@@ -2330,50 +2330,50 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="I32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F33" s="3"/>
       <c r="J33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F34" s="3"/>
       <c r="J34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -2385,7 +2385,7 @@
     <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -2397,7 +2397,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
@@ -2406,50 +2406,50 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="I37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F38" s="3"/>
       <c r="J38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F39" s="3"/>
       <c r="J39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -2461,7 +2461,7 @@
     <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
@@ -2471,73 +2471,73 @@
         <v>13</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F43" s="3"/>
       <c r="I43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="3"/>
       <c r="I44" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
@@ -2547,39 +2547,39 @@
         <v>9</v>
       </c>
       <c r="F45" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I45" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="J45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="3"/>
       <c r="I46" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -2592,28 +2592,28 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F48" s="3"/>
       <c r="I48" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -2622,10 +2622,10 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -2634,15 +2634,15 @@
       </c>
       <c r="F50" s="3"/>
       <c r="H50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
@@ -2651,52 +2651,52 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="I51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J51" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F52" s="3"/>
       <c r="J52" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F53" s="3"/>
       <c r="J53" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2707,10 +2707,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -2719,15 +2719,15 @@
       </c>
       <c r="F55" s="3"/>
       <c r="H55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
@@ -2736,52 +2736,52 @@
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="I56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J56" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F57" s="3"/>
       <c r="J57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F58" s="3"/>
       <c r="J58" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A59" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
@@ -2792,21 +2792,21 @@
       </c>
       <c r="F59" s="3"/>
       <c r="H59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J59" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A60" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A61" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2833,53 +2833,53 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="H62" t="s">
+        <v>165</v>
+      </c>
+      <c r="I62" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="I62" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="J62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E63" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F63" s="3"/>
       <c r="I63" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J63" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A64" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -2888,23 +2888,23 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="H65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
       <c r="B66" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
@@ -2913,23 +2913,23 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="I66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J66" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D67" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="F67" s="3"/>
     </row>
@@ -2937,13 +2937,13 @@
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D68" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="F68" s="3"/>
     </row>
@@ -2951,13 +2951,13 @@
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="F69" s="3"/>
     </row>
@@ -2965,20 +2965,20 @@
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A71" s="3"/>
       <c r="B71" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -2988,7 +2988,7 @@
     <row r="72" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
       <c r="B72" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -2997,49 +2997,49 @@
       </c>
       <c r="F72" s="3"/>
       <c r="H72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I73" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I73" s="9" t="s">
-        <v>183</v>
-      </c>
       <c r="J73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A75" s="3"/>
       <c r="B75" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
@@ -3048,16 +3048,16 @@
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="I75" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J75" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A76" s="3"/>
       <c r="B76" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
@@ -3066,16 +3066,16 @@
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="I76" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A77" s="3"/>
       <c r="B77" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
@@ -3086,16 +3086,16 @@
       </c>
       <c r="F77" s="3"/>
       <c r="I77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J77" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A78" s="3"/>
       <c r="B78" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
@@ -3104,16 +3104,16 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="I78" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A79" s="3"/>
       <c r="B79" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
@@ -3124,16 +3124,16 @@
       </c>
       <c r="F79" s="3"/>
       <c r="I79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J79" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
       <c r="B80" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
@@ -3144,29 +3144,29 @@
       </c>
       <c r="F80" s="3"/>
       <c r="I80" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J80" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A81" s="3"/>
       <c r="B81" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="H81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A82" s="3"/>
       <c r="B82" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
@@ -3177,45 +3177,45 @@
       </c>
       <c r="F82" s="3"/>
       <c r="I82" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J82" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E83" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="I83" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J83" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F84" s="3"/>
       <c r="I84" s="7"/>
@@ -3223,7 +3223,7 @@
     <row r="85" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A85" s="3"/>
       <c r="B85" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
@@ -3234,103 +3234,103 @@
       </c>
       <c r="F85" s="3"/>
       <c r="I85" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J85" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A86" s="3"/>
       <c r="C86" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E86" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F86" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F86" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="I86" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J86" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A87" s="3"/>
       <c r="C87" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F87" s="3"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A88" s="3"/>
       <c r="C88" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F88" s="3"/>
       <c r="I88" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J88" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A89" s="3"/>
       <c r="C89" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I89" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J89" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A90" s="3"/>
       <c r="B90" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="H90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A91" s="3"/>
       <c r="B91" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
@@ -3341,45 +3341,45 @@
       </c>
       <c r="F91" s="3"/>
       <c r="I91" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J91" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E92" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="I92" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J92" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F93" s="3"/>
       <c r="I93" s="7"/>
@@ -3387,7 +3387,7 @@
     <row r="94" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A94" s="3"/>
       <c r="B94" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
@@ -3398,90 +3398,90 @@
       </c>
       <c r="F94" s="3"/>
       <c r="I94" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J94" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A95" s="3"/>
       <c r="C95" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E95" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F95" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F95" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="I95" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J95" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A96" s="3"/>
       <c r="C96" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F96" s="3"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A97" s="3"/>
       <c r="C97" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F97" s="3"/>
       <c r="I97" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J97" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A98" s="3"/>
       <c r="C98" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I98" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J98" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A99" s="3"/>
       <c r="B99" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
@@ -3490,13 +3490,13 @@
       </c>
       <c r="F99" s="3"/>
       <c r="H99" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A100" s="3"/>
       <c r="B100" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -3509,57 +3509,57 @@
       <c r="A101" s="3"/>
       <c r="B101" s="10"/>
       <c r="C101" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F101" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I101" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D101" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E101" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F101" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="I101" s="11" t="s">
-        <v>215</v>
-      </c>
       <c r="J101" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A102" s="3"/>
       <c r="B102" s="10"/>
       <c r="C102" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F102" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="D102" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E102" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F102" s="10" t="s">
+      <c r="I102" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="I102" s="11" t="s">
-        <v>218</v>
-      </c>
       <c r="J102" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A103" s="3"/>
       <c r="B103" s="10"/>
       <c r="C103" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E103" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F103" s="10"/>
       <c r="I103" s="11"/>
@@ -3567,7 +3567,7 @@
     <row r="104" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A104" s="3"/>
       <c r="B104" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C104" s="10"/>
       <c r="D104" s="10" t="s">
@@ -3578,16 +3578,16 @@
       </c>
       <c r="F104" s="10"/>
       <c r="I104" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J104" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A105" s="3"/>
       <c r="B105" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C105" s="10"/>
       <c r="D105" s="10" t="s">
@@ -3598,16 +3598,16 @@
       </c>
       <c r="F105" s="10"/>
       <c r="I105" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J105" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A106" s="3"/>
       <c r="B106" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C106" s="10"/>
       <c r="D106" s="10" t="s">
@@ -3618,16 +3618,16 @@
       </c>
       <c r="F106" s="10"/>
       <c r="I106" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J106" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A107" s="3"/>
       <c r="B107" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="10" t="s">
@@ -3638,16 +3638,16 @@
       </c>
       <c r="F107" s="10"/>
       <c r="I107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J107" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A108" s="3"/>
       <c r="B108" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="10" t="s">
@@ -3658,16 +3658,16 @@
       </c>
       <c r="F108" s="10"/>
       <c r="I108" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J108" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A109" s="3"/>
       <c r="B109" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C109" s="10"/>
       <c r="D109" s="10" t="s">
@@ -3678,16 +3678,16 @@
       </c>
       <c r="F109" s="10"/>
       <c r="I109" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J109" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A110" s="3"/>
       <c r="B110" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="10" t="s">
@@ -3698,16 +3698,16 @@
       </c>
       <c r="F110" s="10"/>
       <c r="I110" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J110" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A111" s="3"/>
       <c r="B111" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
@@ -3716,13 +3716,13 @@
       </c>
       <c r="F111" s="3"/>
       <c r="H111" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A112" s="3"/>
       <c r="B112" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3" t="s">
@@ -3733,16 +3733,16 @@
       </c>
       <c r="F112" s="3"/>
       <c r="I112" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J112" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A113" s="3"/>
       <c r="B113" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
@@ -3754,7 +3754,7 @@
     <row r="114" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A114" s="3"/>
       <c r="B114" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
@@ -3763,35 +3763,35 @@
       </c>
       <c r="F114" s="3"/>
       <c r="H114" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F115" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F115" s="3" t="s">
+      <c r="I115" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="I115" s="4" t="s">
-        <v>242</v>
-      </c>
       <c r="J115" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A116" s="3"/>
       <c r="B116" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
@@ -3802,16 +3802,16 @@
       </c>
       <c r="F116" s="3"/>
       <c r="I116" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J116" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A117" s="3"/>
       <c r="B117" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
@@ -3822,16 +3822,16 @@
       </c>
       <c r="F117" s="3"/>
       <c r="I117" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J117" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A118" s="3"/>
       <c r="B118" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3" t="s">
@@ -3842,16 +3842,16 @@
       </c>
       <c r="F118" s="3"/>
       <c r="I118" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J118" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A119" s="3"/>
       <c r="B119" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
@@ -3862,16 +3862,16 @@
       </c>
       <c r="F119" s="3"/>
       <c r="I119" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J119" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A120" s="3"/>
       <c r="B120" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C120" s="3"/>
       <c r="D120" s="3" t="s">
@@ -3882,16 +3882,16 @@
       </c>
       <c r="F120" s="3"/>
       <c r="I120" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J120" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A121" s="3"/>
       <c r="B121" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C121" s="3"/>
       <c r="D121" s="3" t="s">
@@ -3902,16 +3902,16 @@
       </c>
       <c r="F121" s="3"/>
       <c r="I121" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J121" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A122" s="3"/>
       <c r="B122" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
@@ -3922,41 +3922,41 @@
       </c>
       <c r="F122" s="3"/>
       <c r="I122" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J122" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A123" s="3"/>
       <c r="B123" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F123" s="3"/>
       <c r="H123" t="s">
+        <v>258</v>
+      </c>
+      <c r="I123" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="I123" s="4" t="s">
-        <v>260</v>
-      </c>
       <c r="J123" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="124" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
@@ -3967,10 +3967,10 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A125" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
@@ -3981,56 +3981,56 @@
       </c>
       <c r="F125" s="3"/>
       <c r="H125" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I125" t="s">
+        <v>311</v>
+      </c>
+      <c r="J125" t="s">
         <v>312</v>
-      </c>
-      <c r="J125" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F126" s="3"/>
       <c r="I126" s="4"/>
       <c r="J126" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F127" s="3"/>
       <c r="J127" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A128" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B128" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
@@ -4042,10 +4042,10 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A129" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
@@ -4054,60 +4054,60 @@
       </c>
       <c r="F129" s="3"/>
       <c r="H129" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H130" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I130" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="J130" t="s">
         <v>316</v>
-      </c>
-      <c r="J130" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D131" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D131" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E131" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F131" s="3"/>
       <c r="I131" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J131" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A132" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
@@ -4116,23 +4116,23 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A133" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3"/>
       <c r="H133" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I133" s="12"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B134" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3" t="s">
@@ -4141,67 +4141,67 @@
       <c r="E134" s="3"/>
       <c r="F134" s="3"/>
       <c r="I134" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J134" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B135" s="3"/>
       <c r="C135" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D135" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E135" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="E135" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="F135" s="3"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B136" s="3"/>
       <c r="C136" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D136" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E136" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="E136" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="F136" s="3"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B137" s="3"/>
       <c r="C137" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D137" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="E137" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>177</v>
       </c>
       <c r="F137" s="3"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B138" s="3"/>
       <c r="C138" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B139" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B140" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
@@ -4219,46 +4219,46 @@
       </c>
       <c r="F140" s="3"/>
       <c r="H140" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B141" s="3"/>
       <c r="C141" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I141" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D141" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I141" s="9" t="s">
-        <v>183</v>
-      </c>
       <c r="J141" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B142" s="3"/>
       <c r="C142" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F142" s="3"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B143" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C143" s="3"/>
       <c r="D143" s="3" t="s">
@@ -4267,15 +4267,15 @@
       <c r="E143" s="3"/>
       <c r="F143" s="3"/>
       <c r="I143" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J143" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B144" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
@@ -4284,15 +4284,15 @@
       <c r="E144" s="3"/>
       <c r="F144" s="3"/>
       <c r="I144" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J144" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="145" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B145" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
@@ -4303,15 +4303,15 @@
       </c>
       <c r="F145" s="3"/>
       <c r="I145" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J145" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="146" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B146" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
@@ -4320,15 +4320,15 @@
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
       <c r="I146" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="147" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B147" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
@@ -4339,15 +4339,15 @@
       </c>
       <c r="F147" s="3"/>
       <c r="I147" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J147" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="148" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B148" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C148" s="3"/>
       <c r="D148" s="3" t="s">
@@ -4358,27 +4358,27 @@
       </c>
       <c r="F148" s="3"/>
       <c r="I148" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J148" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="149" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B149" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
       <c r="F149" s="3"/>
       <c r="H149" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="150" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B150" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C150" s="3"/>
       <c r="D150" s="3" t="s">
@@ -4389,50 +4389,50 @@
       </c>
       <c r="F150" s="3"/>
       <c r="I150" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J150" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="151" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B151" s="3"/>
       <c r="C151" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E151" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F151" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F151" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="I151" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J151" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="152" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B152" s="3"/>
       <c r="C152" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F152" s="3"/>
       <c r="I152" s="7"/>
     </row>
     <row r="153" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B153" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C153" s="3"/>
       <c r="D153" s="3" t="s">
@@ -4443,97 +4443,97 @@
       </c>
       <c r="F153" s="3"/>
       <c r="I153" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J153" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="154" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C154" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E154" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F154" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F154" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="I154" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J154" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="155" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C155" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F155" s="3"/>
     </row>
     <row r="156" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C156" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F156" s="3"/>
       <c r="I156" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J156" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="157" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C157" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F157" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D157" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F157" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I157" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J157" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="158" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B158" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
       <c r="F158" s="3"/>
       <c r="H158" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="159" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B159" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C159" s="3"/>
       <c r="D159" s="3" t="s">
@@ -4544,50 +4544,50 @@
       </c>
       <c r="F159" s="3"/>
       <c r="I159" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J159" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="160" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B160" s="3"/>
       <c r="C160" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E160" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F160" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F160" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="I160" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J160" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="161" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B161" s="3"/>
       <c r="C161" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F161" s="3"/>
       <c r="I161" s="7"/>
     </row>
     <row r="162" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B162" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C162" s="3"/>
       <c r="D162" s="3" t="s">
@@ -4598,85 +4598,85 @@
       </c>
       <c r="F162" s="3"/>
       <c r="I162" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J162" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="163" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C163" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E163" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F163" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F163" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="I163" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J163" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="164" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C164" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F164" s="3"/>
     </row>
     <row r="165" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C165" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F165" s="3"/>
       <c r="I165" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J165" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="166" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C166" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F166" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D166" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I166" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J166" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="167" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B167" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
@@ -4685,12 +4685,12 @@
       </c>
       <c r="F167" s="3"/>
       <c r="H167" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="168" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B168" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
@@ -4702,62 +4702,62 @@
     <row r="169" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B169" s="10"/>
       <c r="C169" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D169" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E169" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F169" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I169" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="D169" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E169" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F169" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="I169" s="11" t="s">
-        <v>215</v>
-      </c>
       <c r="J169" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="170" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B170" s="10"/>
       <c r="C170" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D170" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E170" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F170" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="D170" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E170" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F170" s="10" t="s">
+      <c r="I170" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="I170" s="11" t="s">
-        <v>218</v>
-      </c>
       <c r="J170" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="171" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B171" s="10"/>
       <c r="C171" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D171" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E171" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F171" s="10"/>
       <c r="I171" s="11"/>
     </row>
     <row r="172" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B172" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10" t="s">
@@ -4768,15 +4768,15 @@
       </c>
       <c r="F172" s="10"/>
       <c r="I172" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J172" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="173" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B173" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C173" s="10"/>
       <c r="D173" s="10" t="s">
@@ -4787,15 +4787,15 @@
       </c>
       <c r="F173" s="10"/>
       <c r="I173" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J173" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="174" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B174" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C174" s="10"/>
       <c r="D174" s="10" t="s">
@@ -4806,15 +4806,15 @@
       </c>
       <c r="F174" s="10"/>
       <c r="I174" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J174" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="175" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B175" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C175" s="10"/>
       <c r="D175" s="10" t="s">
@@ -4825,15 +4825,15 @@
       </c>
       <c r="F175" s="10"/>
       <c r="I175" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J175" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="176" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B176" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C176" s="10"/>
       <c r="D176" s="10" t="s">
@@ -4844,15 +4844,15 @@
       </c>
       <c r="F176" s="10"/>
       <c r="I176" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J176" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B177" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="10" t="s">
@@ -4863,15 +4863,15 @@
       </c>
       <c r="F177" s="10"/>
       <c r="I177" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J177" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B178" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C178" s="10"/>
       <c r="D178" s="10" t="s">
@@ -4882,15 +4882,15 @@
       </c>
       <c r="F178" s="10"/>
       <c r="I178" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J178" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B179" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C179" s="3"/>
       <c r="D179" s="3"/>
@@ -4899,12 +4899,12 @@
       </c>
       <c r="F179" s="3"/>
       <c r="H179" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B180" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C180" s="3"/>
       <c r="D180" s="3" t="s">
@@ -4915,15 +4915,15 @@
       </c>
       <c r="F180" s="3"/>
       <c r="I180" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J180" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B181" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C181" s="3"/>
       <c r="D181" s="3"/>
@@ -4934,7 +4934,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B182" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C182" s="3"/>
       <c r="D182" s="3"/>
@@ -4943,33 +4943,33 @@
       </c>
       <c r="F182" s="3"/>
       <c r="H182" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B183" s="3"/>
       <c r="C183" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F183" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D183" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E183" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F183" s="3" t="s">
+      <c r="I183" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="I183" s="4" t="s">
-        <v>242</v>
-      </c>
       <c r="J183" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B184" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C184" s="3"/>
       <c r="D184" s="3" t="s">
@@ -4980,15 +4980,15 @@
       </c>
       <c r="F184" s="3"/>
       <c r="I184" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J184" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B185" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C185" s="3"/>
       <c r="D185" s="3" t="s">
@@ -4999,15 +4999,15 @@
       </c>
       <c r="F185" s="3"/>
       <c r="I185" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J185" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B186" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
@@ -5018,15 +5018,15 @@
       </c>
       <c r="F186" s="3"/>
       <c r="I186" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J186" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B187" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C187" s="3"/>
       <c r="D187" s="3" t="s">
@@ -5037,15 +5037,15 @@
       </c>
       <c r="F187" s="3"/>
       <c r="I187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J187" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B188" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C188" s="3"/>
       <c r="D188" s="3" t="s">
@@ -5056,15 +5056,15 @@
       </c>
       <c r="F188" s="3"/>
       <c r="I188" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J188" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B189" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C189" s="3"/>
       <c r="D189" s="3" t="s">
@@ -5075,15 +5075,15 @@
       </c>
       <c r="F189" s="3"/>
       <c r="I189" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J189" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B190" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C190" s="3"/>
       <c r="D190" s="3" t="s">
@@ -5094,65 +5094,65 @@
       </c>
       <c r="F190" s="3"/>
       <c r="I190" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J190" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B191" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C191" s="3"/>
       <c r="D191" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F191" s="3"/>
       <c r="H191" t="s">
+        <v>258</v>
+      </c>
+      <c r="I191" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="I191" s="4" t="s">
-        <v>260</v>
-      </c>
       <c r="J191" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="192" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A192" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B192" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="C192" s="3"/>
       <c r="D192" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E192" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F192" s="3"/>
       <c r="H192" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I192" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="J192" t="s">
         <v>357</v>
-      </c>
-      <c r="J192" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A193" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B193" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C193" s="3"/>
       <c r="D193" s="3" t="s">
@@ -5163,18 +5163,18 @@
       </c>
       <c r="F193" s="3"/>
       <c r="I193" t="s">
+        <v>358</v>
+      </c>
+      <c r="J193" t="s">
         <v>359</v>
-      </c>
-      <c r="J193" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A194" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C194" s="3"/>
       <c r="D194" s="3"/>
@@ -5185,10 +5185,10 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A195" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C195" s="3"/>
       <c r="D195" s="3"/>
@@ -5197,21 +5197,21 @@
       </c>
       <c r="F195" s="3"/>
       <c r="H195" t="s">
+        <v>360</v>
+      </c>
+      <c r="I195" t="s">
         <v>361</v>
       </c>
-      <c r="I195" t="s">
+      <c r="J195" t="s">
         <v>362</v>
-      </c>
-      <c r="J195" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A196" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B196" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C196" s="3"/>
       <c r="D196" s="3" t="s">
@@ -5222,18 +5222,18 @@
       </c>
       <c r="F196" s="3"/>
       <c r="H196" t="s">
+        <v>261</v>
+      </c>
+      <c r="I196" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="I196" s="4" t="s">
-        <v>263</v>
-      </c>
       <c r="J196" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B199" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>